<commit_message>
fix RL verify cost
</commit_message>
<xml_diff>
--- a/Smart_Nodes_Routing/experiments/Evaluations_v2.xlsx
+++ b/Smart_Nodes_Routing/experiments/Evaluations_v2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IdoYe\PycharmProjects\Research_Implementing\Smart_Nodes_Routing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IdoYe\PycharmProjects\Research_Implementing\Smart_Nodes_Routing\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10918DEA-2830-4878-A229-DC4389C3759E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934AE08B-F62C-4384-83BB-D2993D6A1181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="4" xr2:uid="{F03132DC-CDBD-427F-ACA0-8693D7E39B80}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="122">
   <si>
     <t>Number of Nodes</t>
   </si>
@@ -387,6 +387,24 @@
   <si>
     <t>4 Smart Node                 (0, 4, 9, 13) 20.3526</t>
   </si>
+  <si>
+    <t xml:space="preserve"> G_1 (1.0,0.1)  G_2 (0.1,0.01)</t>
+  </si>
+  <si>
+    <t>1 Smart Node       (39,) 1.07204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Smart Node        (8, 39, 28) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Smart Node                 (8, 39, 27, 28) </t>
+  </si>
+  <si>
+    <t>5 Smart Node                 (8, 18, 27, 28, 39)</t>
+  </si>
+  <si>
+    <t>2 Smart Node      (39, 28) 1.07381</t>
+  </si>
 </sst>
 </file>
 
@@ -503,7 +521,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
@@ -614,6 +632,17 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -36550,10 +36579,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11AED99B-294B-42C3-BD53-BEA0C0BE6E68}">
-  <dimension ref="A1:AD71"/>
+  <dimension ref="A1:AD111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37375,13 +37404,33 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="G12" s="10">
-        <f>AVERAGE(G5:G11)</f>
-        <v>4.7288460696611904E-4</v>
+        <f>AVERAGE(G7:G11)</f>
+        <v>5.3163500281763201E-4</v>
       </c>
       <c r="H12" s="21"/>
       <c r="I12" s="10">
         <f>AVERAGE(I5:I11)</f>
         <v>0.12725075081989862</v>
+      </c>
+      <c r="O12" s="37">
+        <f>AVERAGE(O7:O11)</f>
+        <v>3.066721078957091E-3</v>
+      </c>
+      <c r="Q12" s="37">
+        <f>AVERAGE(Q7:Q11)</f>
+        <v>6.1956075743792023E-4</v>
+      </c>
+      <c r="S12" s="37">
+        <f>AVERAGE(S7:S11)</f>
+        <v>2.7328291132623582E-3</v>
+      </c>
+      <c r="U12" s="37">
+        <f>AVERAGE(U7:U11)</f>
+        <v>3.043628574307222E-3</v>
+      </c>
+      <c r="W12" s="37">
+        <f>AVERAGE(W7:W11)</f>
+        <v>4.8086813537807863E-3</v>
       </c>
       <c r="Z12" s="12"/>
       <c r="AA12" s="12"/>
@@ -38386,14 +38435,725 @@
       </c>
     </row>
     <row r="71" spans="20:27" x14ac:dyDescent="0.25">
-      <c r="T71" s="45"/>
-      <c r="U71" s="45"/>
-      <c r="V71" s="45"/>
-      <c r="W71" s="45"/>
-      <c r="X71" s="45"/>
-      <c r="Y71" s="45"/>
-      <c r="Z71" s="45"/>
-      <c r="AA71" s="45"/>
+      <c r="T71" s="46"/>
+      <c r="U71" s="46"/>
+      <c r="V71" s="46"/>
+      <c r="W71" s="46"/>
+      <c r="X71" s="46"/>
+      <c r="Y71" s="46"/>
+      <c r="Z71" s="46"/>
+      <c r="AA71" s="46"/>
+    </row>
+    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A100" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B100" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C100" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D100" s="45"/>
+      <c r="E100" s="45"/>
+      <c r="F100" s="45"/>
+      <c r="G100" s="45"/>
+      <c r="H100" s="45"/>
+      <c r="I100" s="45"/>
+      <c r="J100" s="45"/>
+      <c r="K100" s="45"/>
+      <c r="L100" s="45"/>
+      <c r="M100" s="45"/>
+      <c r="N100" s="45"/>
+      <c r="O100" s="45"/>
+      <c r="P100" s="45"/>
+      <c r="Q100" s="45"/>
+      <c r="R100" s="45"/>
+      <c r="S100" s="45"/>
+      <c r="T100" s="45"/>
+      <c r="U100" s="45"/>
+      <c r="V100" s="45"/>
+      <c r="W100" s="45"/>
+      <c r="X100" s="45"/>
+      <c r="Y100" s="45"/>
+    </row>
+    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A101" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B101" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="C101" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="D101" s="45"/>
+      <c r="E101" s="45"/>
+      <c r="F101" s="45"/>
+      <c r="G101" s="45"/>
+      <c r="H101" s="45"/>
+      <c r="I101" s="45"/>
+      <c r="J101" s="45"/>
+      <c r="K101" s="45"/>
+      <c r="L101" s="45"/>
+      <c r="M101" s="45"/>
+      <c r="N101" s="45"/>
+      <c r="O101" s="45"/>
+      <c r="P101" s="45"/>
+      <c r="Q101" s="45"/>
+      <c r="R101" s="45"/>
+      <c r="S101" s="45"/>
+      <c r="T101" s="45"/>
+      <c r="U101" s="45"/>
+      <c r="V101" s="45"/>
+      <c r="W101" s="45"/>
+      <c r="X101" s="45"/>
+      <c r="Y101" s="45"/>
+    </row>
+    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A102" s="45"/>
+      <c r="B102" s="45"/>
+      <c r="C102" s="45"/>
+      <c r="D102" s="45"/>
+      <c r="E102" s="45"/>
+      <c r="F102" s="45"/>
+      <c r="G102" s="45"/>
+      <c r="H102" s="45"/>
+      <c r="I102" s="45"/>
+      <c r="J102" s="45"/>
+      <c r="K102" s="45"/>
+      <c r="L102" s="45"/>
+      <c r="M102" s="45"/>
+      <c r="N102" s="45"/>
+      <c r="O102" s="45"/>
+      <c r="P102" s="45"/>
+      <c r="Q102" s="45"/>
+      <c r="R102" s="45"/>
+      <c r="S102" s="45"/>
+      <c r="T102" s="45"/>
+      <c r="U102" s="45"/>
+      <c r="V102" s="45"/>
+      <c r="W102" s="45"/>
+      <c r="X102" s="45"/>
+      <c r="Y102" s="45"/>
+    </row>
+    <row r="103" spans="1:25" ht="90" x14ac:dyDescent="0.25">
+      <c r="A103" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B103" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C103" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="D103" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="E103" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="F103" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="G103" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="H103" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="I103" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="J103" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="K103" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="L103" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="M103" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="N103" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="O103" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="P103" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q103" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="R103" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="S103" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="T103" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="U103" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="V103" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="W103" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="X103" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y103" s="41" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="104" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A104" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B104" s="40">
+        <v>1024</v>
+      </c>
+      <c r="C104" s="15">
+        <v>1.0691673920487901</v>
+      </c>
+      <c r="D104" s="42">
+        <v>1.93579677443327</v>
+      </c>
+      <c r="E104" s="50">
+        <f>D104/C104-1</f>
+        <v>0.81056473366981674</v>
+      </c>
+      <c r="F104" s="42">
+        <v>1.06920863769149</v>
+      </c>
+      <c r="G104" s="31">
+        <f>F104/C104-1</f>
+        <v>3.857734813705882E-5</v>
+      </c>
+      <c r="H104" s="40">
+        <v>1.1825000000000001</v>
+      </c>
+      <c r="I104" s="47">
+        <f>H104/C104-1</f>
+        <v>0.10600080847400006</v>
+      </c>
+      <c r="J104" s="42">
+        <v>1.0788928364514501</v>
+      </c>
+      <c r="K104" s="11">
+        <f>J104/C104-1</f>
+        <v>9.0962785387829204E-3</v>
+      </c>
+      <c r="L104" s="15">
+        <v>1.0763</v>
+      </c>
+      <c r="M104" s="11">
+        <f>L104/C104-1</f>
+        <v>6.6711798398022548E-3</v>
+      </c>
+      <c r="N104" s="15">
+        <v>1.07149196666666</v>
+      </c>
+      <c r="O104" s="11">
+        <f>N104/C104-1</f>
+        <v>2.1741914644586302E-3</v>
+      </c>
+      <c r="P104" s="15"/>
+      <c r="Q104" s="11">
+        <f>P104/C104-1</f>
+        <v>-1</v>
+      </c>
+      <c r="R104" s="15"/>
+      <c r="S104" s="48">
+        <f>R104/C104-1</f>
+        <v>-1</v>
+      </c>
+      <c r="T104" s="15"/>
+      <c r="U104" s="11">
+        <f>T104/C104-1</f>
+        <v>-1</v>
+      </c>
+      <c r="V104" s="15"/>
+      <c r="W104" s="11">
+        <f>V104/C104-1</f>
+        <v>-1</v>
+      </c>
+      <c r="X104" s="39"/>
+      <c r="Y104" s="49">
+        <f>X104/C104-1</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A105" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B105" s="40">
+        <v>4096</v>
+      </c>
+      <c r="C105" s="15">
+        <v>1.06878744438038</v>
+      </c>
+      <c r="D105" s="42">
+        <v>2.0092871822281202</v>
+      </c>
+      <c r="E105" s="50">
+        <f t="shared" ref="E105:E110" si="24">D105/C105-1</f>
+        <v>0.87996892440384777</v>
+      </c>
+      <c r="F105" s="42">
+        <v>1.0689557857980101</v>
+      </c>
+      <c r="G105" s="31">
+        <f t="shared" ref="G105" si="25">F105/C105-1</f>
+        <v>1.5750691918703374E-4</v>
+      </c>
+      <c r="H105" s="40">
+        <v>1.1890000000000001</v>
+      </c>
+      <c r="I105" s="47">
+        <f t="shared" ref="I105" si="26">H105/C105-1</f>
+        <v>0.11247564354511308</v>
+      </c>
+      <c r="J105" s="42">
+        <v>1.0803951859875001</v>
+      </c>
+      <c r="K105" s="11">
+        <f t="shared" ref="K105:K110" si="27">J105/C105-1</f>
+        <v>1.0860664267860587E-2</v>
+      </c>
+      <c r="L105" s="15">
+        <v>1.0722</v>
+      </c>
+      <c r="M105" s="11">
+        <f t="shared" ref="M105:M110" si="28">L105/C105-1</f>
+        <v>3.192922631682249E-3</v>
+      </c>
+      <c r="N105" s="19">
+        <v>1.0668331</v>
+      </c>
+      <c r="O105" s="11">
+        <f t="shared" ref="O105:O110" si="29">N105/C105-1</f>
+        <v>-1.8285622559057746E-3</v>
+      </c>
+      <c r="P105" s="19"/>
+      <c r="Q105" s="11">
+        <f t="shared" ref="Q105:Q110" si="30">P105/C105-1</f>
+        <v>-1</v>
+      </c>
+      <c r="R105" s="19"/>
+      <c r="S105" s="48">
+        <f t="shared" ref="S105:S110" si="31">R105/C105-1</f>
+        <v>-1</v>
+      </c>
+      <c r="T105" s="15"/>
+      <c r="U105" s="11">
+        <f>T105/C105-1</f>
+        <v>-1</v>
+      </c>
+      <c r="V105" s="15"/>
+      <c r="W105" s="11">
+        <f t="shared" ref="W105:W110" si="32">V105/C105-1</f>
+        <v>-1</v>
+      </c>
+      <c r="X105" s="39"/>
+      <c r="Y105" s="49">
+        <f t="shared" ref="Y105:Y110" si="33">X105/C105-1</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A106" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B106" s="40">
+        <v>1024</v>
+      </c>
+      <c r="C106" s="15">
+        <v>1.080916452196</v>
+      </c>
+      <c r="D106" s="42">
+        <v>1.9268789942761999</v>
+      </c>
+      <c r="E106" s="50">
+        <f t="shared" si="24"/>
+        <v>0.78263453235588609</v>
+      </c>
+      <c r="F106" s="42">
+        <v>1.0809228225834899</v>
+      </c>
+      <c r="G106" s="31">
+        <f>F106/C106-1</f>
+        <v>5.8935059015219338E-6</v>
+      </c>
+      <c r="H106" s="40">
+        <v>1.1833</v>
+      </c>
+      <c r="I106" s="47">
+        <f>H106/C106-1</f>
+        <v>9.471920572214132E-2</v>
+      </c>
+      <c r="J106" s="42">
+        <v>1.0904654043514099</v>
+      </c>
+      <c r="K106" s="11">
+        <f t="shared" si="27"/>
+        <v>8.8341260196476146E-3</v>
+      </c>
+      <c r="L106" s="40">
+        <v>1.0818000000000001</v>
+      </c>
+      <c r="M106" s="11">
+        <f t="shared" si="28"/>
+        <v>8.1740619472037146E-4</v>
+      </c>
+      <c r="N106" s="19"/>
+      <c r="O106" s="11">
+        <f t="shared" si="29"/>
+        <v>-1</v>
+      </c>
+      <c r="P106" s="19"/>
+      <c r="Q106" s="11">
+        <f t="shared" si="30"/>
+        <v>-1</v>
+      </c>
+      <c r="R106" s="19"/>
+      <c r="S106" s="48">
+        <f t="shared" si="31"/>
+        <v>-1</v>
+      </c>
+      <c r="T106" s="19"/>
+      <c r="U106" s="11">
+        <f t="shared" ref="U106:U110" si="34">T106/C106-1</f>
+        <v>-1</v>
+      </c>
+      <c r="V106" s="19"/>
+      <c r="W106" s="11">
+        <f t="shared" si="32"/>
+        <v>-1</v>
+      </c>
+      <c r="X106" s="39">
+        <v>1.1151</v>
+      </c>
+      <c r="Y106" s="49">
+        <f t="shared" si="33"/>
+        <v>3.1624597566770607E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A107" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B107" s="40">
+        <v>1024</v>
+      </c>
+      <c r="C107" s="15">
+        <v>1.0781284516037599</v>
+      </c>
+      <c r="D107" s="42">
+        <v>1.87418921316641</v>
+      </c>
+      <c r="E107" s="50">
+        <f t="shared" si="24"/>
+        <v>0.7383728352391381</v>
+      </c>
+      <c r="F107" s="42">
+        <v>1.0782453306467901</v>
+      </c>
+      <c r="G107" s="31">
+        <f>F107/C107-1</f>
+        <v>1.0840920008758914E-4</v>
+      </c>
+      <c r="H107" s="40">
+        <v>1.1921999999999999</v>
+      </c>
+      <c r="I107" s="47">
+        <f>H107/C107-1</f>
+        <v>0.10580515543074109</v>
+      </c>
+      <c r="J107" s="42">
+        <v>1.0886813532578501</v>
+      </c>
+      <c r="K107" s="11">
+        <f t="shared" si="27"/>
+        <v>9.7881672989821311E-3</v>
+      </c>
+      <c r="L107" s="40">
+        <v>1.0843</v>
+      </c>
+      <c r="M107" s="11">
+        <f t="shared" si="28"/>
+        <v>5.7243164180109662E-3</v>
+      </c>
+      <c r="N107" s="19"/>
+      <c r="O107" s="11">
+        <f t="shared" si="29"/>
+        <v>-1</v>
+      </c>
+      <c r="P107" s="19"/>
+      <c r="Q107" s="11">
+        <f t="shared" si="30"/>
+        <v>-1</v>
+      </c>
+      <c r="R107" s="19"/>
+      <c r="S107" s="48">
+        <f t="shared" si="31"/>
+        <v>-1</v>
+      </c>
+      <c r="T107" s="19"/>
+      <c r="U107" s="11">
+        <f t="shared" si="34"/>
+        <v>-1</v>
+      </c>
+      <c r="V107" s="19"/>
+      <c r="W107" s="11">
+        <f t="shared" si="32"/>
+        <v>-1</v>
+      </c>
+      <c r="X107" s="39"/>
+      <c r="Y107" s="49">
+        <f t="shared" si="33"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A108" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="B108" s="40">
+        <v>1024</v>
+      </c>
+      <c r="C108" s="15">
+        <v>1.07553314350806</v>
+      </c>
+      <c r="D108" s="42">
+        <v>1.08698764621011</v>
+      </c>
+      <c r="E108" s="50">
+        <f t="shared" si="24"/>
+        <v>1.0650069475952151E-2</v>
+      </c>
+      <c r="F108" s="42">
+        <v>1.07562159275873</v>
+      </c>
+      <c r="G108" s="31">
+        <f>F108/C108-1</f>
+        <v>8.2237587194722295E-5</v>
+      </c>
+      <c r="H108" s="40">
+        <v>1.1903999999999999</v>
+      </c>
+      <c r="I108" s="47">
+        <f>H108/C108-1</f>
+        <v>0.10679992261073368</v>
+      </c>
+      <c r="J108" s="42">
+        <v>1.08663525410107</v>
+      </c>
+      <c r="K108" s="11">
+        <f t="shared" si="27"/>
+        <v>1.0322425357156773E-2</v>
+      </c>
+      <c r="L108" s="40">
+        <v>1.07605</v>
+      </c>
+      <c r="M108" s="11">
+        <f t="shared" si="28"/>
+        <v>4.8055840497318592E-4</v>
+      </c>
+      <c r="N108" s="15"/>
+      <c r="O108" s="11">
+        <f t="shared" si="29"/>
+        <v>-1</v>
+      </c>
+      <c r="P108" s="19"/>
+      <c r="Q108" s="11">
+        <f t="shared" si="30"/>
+        <v>-1</v>
+      </c>
+      <c r="R108" s="19"/>
+      <c r="S108" s="48">
+        <f t="shared" si="31"/>
+        <v>-1</v>
+      </c>
+      <c r="T108" s="15"/>
+      <c r="U108" s="11">
+        <f t="shared" si="34"/>
+        <v>-1</v>
+      </c>
+      <c r="V108" s="15"/>
+      <c r="W108" s="11">
+        <f t="shared" si="32"/>
+        <v>-1</v>
+      </c>
+      <c r="X108" s="39"/>
+      <c r="Y108" s="49">
+        <f t="shared" si="33"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A109" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B109" s="40">
+        <v>1024</v>
+      </c>
+      <c r="C109" s="15">
+        <v>1.0647976994965</v>
+      </c>
+      <c r="D109" s="42">
+        <v>1.0749073471420401</v>
+      </c>
+      <c r="E109" s="50">
+        <f t="shared" si="24"/>
+        <v>9.4944303977371192E-3</v>
+      </c>
+      <c r="F109" s="42">
+        <v>1.0653177246936101</v>
+      </c>
+      <c r="G109" s="31">
+        <f>F109/C109-1</f>
+        <v>4.8837933943324252E-4</v>
+      </c>
+      <c r="H109" s="40">
+        <v>1.1862999999999999</v>
+      </c>
+      <c r="I109" s="47">
+        <f>H109/C109-1</f>
+        <v>0.11410834242124435</v>
+      </c>
+      <c r="J109" s="42">
+        <v>1.07587025743599</v>
+      </c>
+      <c r="K109" s="11">
+        <f t="shared" si="27"/>
+        <v>1.039874329623891E-2</v>
+      </c>
+      <c r="L109" s="40">
+        <v>1.073</v>
+      </c>
+      <c r="M109" s="11">
+        <f t="shared" si="28"/>
+        <v>7.7031538548386624E-3</v>
+      </c>
+      <c r="N109" s="15"/>
+      <c r="O109" s="11">
+        <f t="shared" si="29"/>
+        <v>-1</v>
+      </c>
+      <c r="P109" s="19"/>
+      <c r="Q109" s="11">
+        <f t="shared" si="30"/>
+        <v>-1</v>
+      </c>
+      <c r="R109" s="16"/>
+      <c r="S109" s="48">
+        <f t="shared" si="31"/>
+        <v>-1</v>
+      </c>
+      <c r="T109" s="15"/>
+      <c r="U109" s="11">
+        <f t="shared" si="34"/>
+        <v>-1</v>
+      </c>
+      <c r="V109" s="15"/>
+      <c r="W109" s="11">
+        <f t="shared" si="32"/>
+        <v>-1</v>
+      </c>
+      <c r="X109" s="39"/>
+      <c r="Y109" s="49">
+        <f t="shared" si="33"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A110" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="B110" s="40">
+        <v>1024</v>
+      </c>
+      <c r="C110" s="15">
+        <v>1.06537601855421</v>
+      </c>
+      <c r="D110" s="42">
+        <v>1.08186152605863</v>
+      </c>
+      <c r="E110" s="50">
+        <f t="shared" si="24"/>
+        <v>1.5473886418798877E-2</v>
+      </c>
+      <c r="F110" s="42">
+        <v>1.0654982698511699</v>
+      </c>
+      <c r="G110" s="31">
+        <f>F110/C110-1</f>
+        <v>1.1474943572098439E-4</v>
+      </c>
+      <c r="H110" s="40">
+        <v>1.1865000000000001</v>
+      </c>
+      <c r="I110" s="47">
+        <f>H110/C110-1</f>
+        <v>0.11369129709730452</v>
+      </c>
+      <c r="J110" s="42">
+        <v>1.0752062428758999</v>
+      </c>
+      <c r="K110" s="11">
+        <f t="shared" si="27"/>
+        <v>9.2269998108556184E-3</v>
+      </c>
+      <c r="L110" s="40">
+        <v>1.0696000000000001</v>
+      </c>
+      <c r="M110" s="11">
+        <f t="shared" si="28"/>
+        <v>3.9647799201658618E-3</v>
+      </c>
+      <c r="N110" s="15"/>
+      <c r="O110" s="11">
+        <f t="shared" si="29"/>
+        <v>-1</v>
+      </c>
+      <c r="P110" s="15"/>
+      <c r="Q110" s="11">
+        <f t="shared" si="30"/>
+        <v>-1</v>
+      </c>
+      <c r="R110" s="15"/>
+      <c r="S110" s="48">
+        <f t="shared" si="31"/>
+        <v>-1</v>
+      </c>
+      <c r="T110" s="15"/>
+      <c r="U110" s="11">
+        <f t="shared" si="34"/>
+        <v>-1</v>
+      </c>
+      <c r="V110" s="15"/>
+      <c r="W110" s="11">
+        <f t="shared" si="32"/>
+        <v>-1</v>
+      </c>
+      <c r="X110" s="39"/>
+      <c r="Y110" s="49">
+        <f t="shared" si="33"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="M111" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>